<commit_message>
Added boundary condition to table
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_short.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_short.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>PDE_model</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Mesh_type</t>
   </si>
   <si>
+    <t>Boundary_condition</t>
+  </si>
+  <si>
     <t>Scheme_order</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
     <t>Regular_RightTriangles</t>
   </si>
   <si>
+    <t>Dirichlet</t>
+  </si>
+  <si>
     <t>Triangles</t>
   </si>
   <si>
@@ -75,6 +81,9 @@
   </si>
   <si>
     <t>Squares</t>
+  </si>
+  <si>
+    <t>Neumann</t>
   </si>
   <si>
     <t>Orange(order 0)</t>
@@ -435,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +452,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,382 +477,424 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="n">
         <v>2.003941254089581</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="n">
-        <v>119.5647480487823</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="n">
+        <v>109.4771571159363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.015608644460145</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="n">
-        <v>2.015608644460145</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="n">
-        <v>6.094477891921997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6.233874082565308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="n">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.340336836145038</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="n">
-        <v>208.4592311382294</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="n">
+        <v>208.5218908786774</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.6690820358074518</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
       <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="n">
-        <v>11.90931582450867</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="n">
+        <v>12.18183302879333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
         <v>2.003941213535303</v>
       </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
       <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="n">
-        <v>9.851321935653687</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="n">
+        <v>10.15054607391357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="n">
         <v>2.003941211551183</v>
       </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
       <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="n">
-        <v>9.898462057113647</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="n">
+        <v>9.985594987869263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
         <v>0.02119663100406134</v>
       </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
       <c r="H8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="n">
-        <v>15.68182492256165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>13</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="n">
+        <v>18.92783284187317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="n">
         <v>-0.005617740418916485</v>
       </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
       <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="n">
-        <v>15.86531114578247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="n">
+        <v>18.37629008293152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="n">
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.8952237869134417</v>
       </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
       <c r="H10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" t="n">
-        <v>4.744688034057617</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4.93955397605896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
         <v>2</v>
       </c>
       <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.6137798580984465</v>
+      </c>
+      <c r="H11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.6137798580984465</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2.505467891693115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2.616051912307739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" t="n">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
         <v>1.340336836132099</v>
       </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
       <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" t="n">
-        <v>5.868787050247192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5.918725967407227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" t="n">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.006535470643459771</v>
       </c>
-      <c r="G13" t="s">
-        <v>15</v>
-      </c>
       <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" t="n">
-        <v>62.12639307975769</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="n">
+        <v>64.21971893310547</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D14" t="n">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="n">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.5358788100873692</v>
       </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
       <c r="H14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" t="n">
-        <v>3.679362773895264</v>
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3.755897998809814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated convergence table with short labels
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_short.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_short.xlsx
@@ -20,16 +20,16 @@
     <t>PDE_model</t>
   </si>
   <si>
-    <t>Numerical_method_name</t>
-  </si>
-  <si>
-    <t>Mesh_dimension</t>
+    <t>Num_method</t>
+  </si>
+  <si>
+    <t>Mesh_dim</t>
   </si>
   <si>
     <t>Mesh_type</t>
   </si>
   <si>
-    <t>Boundary_condition</t>
+    <t>Bound_cond</t>
   </si>
   <si>
     <t>Scheme_order</t>
@@ -41,7 +41,7 @@
     <t>Test_color</t>
   </si>
   <si>
-    <t>Computational_time</t>
+    <t>Comput_time</t>
   </si>
   <si>
     <t>Poisson</t>
@@ -89,13 +89,13 @@
     <t>Orange(order 0)</t>
   </si>
   <si>
+    <t>Regular_Cubes</t>
+  </si>
+  <si>
+    <t>Cubes</t>
+  </si>
+  <si>
     <t>Structured_triangles</t>
-  </si>
-  <si>
-    <t>Regular_Cubes</t>
-  </si>
-  <si>
-    <t>Cubes</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="n">
-        <v>2.003941254089581</v>
+        <v>2.0039</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -510,7 +510,7 @@
         <v>14</v>
       </c>
       <c r="J2" t="n">
-        <v>109.4771571159363</v>
+        <v>108.1455399990082</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="G3" t="n">
-        <v>2.015608644460145</v>
+        <v>2.0156</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="J3" t="n">
-        <v>6.233874082565308</v>
+        <v>6.762243032455444</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="G4" t="n">
-        <v>1.340336836145038</v>
+        <v>1.3403</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
@@ -574,7 +574,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="n">
-        <v>208.5218908786774</v>
+        <v>210.4683861732483</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -597,7 +597,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6690820358074518</v>
+        <v>0.6691</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -606,7 +606,7 @@
         <v>14</v>
       </c>
       <c r="J5" t="n">
-        <v>12.18183302879333</v>
+        <v>11.9149010181427</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -629,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="n">
-        <v>2.003941213535303</v>
+        <v>2.0039</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
@@ -638,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="J6" t="n">
-        <v>10.15054607391357</v>
+        <v>9.832487106323242</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -661,7 +661,7 @@
         <v>22</v>
       </c>
       <c r="G7" t="n">
-        <v>2.003941211551183</v>
+        <v>2.0039</v>
       </c>
       <c r="H7" t="s">
         <v>21</v>
@@ -670,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="J7" t="n">
-        <v>9.985594987869263</v>
+        <v>9.859630107879639</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -693,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="n">
-        <v>0.02119663100406134</v>
+        <v>0.0212</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -702,7 +702,7 @@
         <v>14</v>
       </c>
       <c r="J8" t="n">
-        <v>18.92783284187317</v>
+        <v>15.65501999855042</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -725,7 +725,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.005617740418916485</v>
+        <v>-0.0056</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
@@ -734,12 +734,12 @@
         <v>23</v>
       </c>
       <c r="J9" t="n">
-        <v>18.37629008293152</v>
+        <v>15.78992199897766</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -751,13 +751,13 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8952237869134417</v>
+        <v>0.6138</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -766,12 +766,12 @@
         <v>14</v>
       </c>
       <c r="J10" t="n">
-        <v>4.93955397605896</v>
+        <v>2.600184917449951</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -780,30 +780,28 @@
         <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F11" t="s"/>
       <c r="G11" t="n">
-        <v>0.6137798580984465</v>
+        <v>1.3403</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I11" t="s">
         <v>14</v>
       </c>
       <c r="J11" t="n">
-        <v>2.616051912307739</v>
+        <v>5.900697946548462</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -815,27 +813,27 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="n">
-        <v>1.340336836132099</v>
+        <v>0.0065</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
       </c>
       <c r="J12" t="n">
-        <v>5.918725967407227</v>
+        <v>62.56098890304565</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -847,13 +845,13 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
       <c r="G13" t="n">
-        <v>0.006535470643459771</v>
+        <v>0.5359</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
@@ -862,39 +860,37 @@
         <v>14</v>
       </c>
       <c r="J13" t="n">
-        <v>64.21971893310547</v>
+        <v>3.782500028610229</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
+      <c r="C14" t="s"/>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5358788100873692</v>
+        <v>0.8952</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I14" t="s">
         <v>14</v>
       </c>
       <c r="J14" t="n">
-        <v>3.755897998809814</v>
+        <v>4.790747165679932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>